<commit_message>
feat: add calendar module
</commit_message>
<xml_diff>
--- a/график.xlsx
+++ b/график.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Soft\Projects\duty-days\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07A42DDD-308A-4CC8-B47C-59C77E0AD933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAA547E-25CB-45CB-9CF6-4D2A33628DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{06CC82AA-A849-49A9-B537-A57D398D68E9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Организация</t>
   </si>
@@ -101,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -395,13 +395,13 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -727,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3614CDEF-5A3B-4DF8-81A4-29A2F706B2DE}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18:L19"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,6 +927,25 @@
         <v>89543512312</v>
       </c>
     </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="19">
+        <v>45659</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="13">
+        <v>89543512312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat(item): add services logic
</commit_message>
<xml_diff>
--- a/график.xlsx
+++ b/график.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Soft\Projects\duty-days\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Soft\Projects\duty-calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4730F71-BB67-4C0E-8739-D24E814AF991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E354B5CF-2B24-49CD-AFA7-F92EAC7D3FF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{06CC82AA-A849-49A9-B537-A57D398D68E9}"/>
+    <workbookView xWindow="3075" yWindow="3105" windowWidth="21600" windowHeight="13185" xr2:uid="{06CC82AA-A849-49A9-B537-A57D398D68E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Организация</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Зам. Главы администрации</t>
+  </si>
+  <si>
+    <t>Председатель, ДС</t>
+  </si>
+  <si>
+    <t>Латинская Татьяна Николаевна</t>
+  </si>
+  <si>
+    <t>Оперативный дежурный</t>
   </si>
 </sst>
 </file>
@@ -121,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -353,11 +362,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -414,6 +449,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -728,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3614CDEF-5A3B-4DF8-81A4-29A2F706B2DE}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +999,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="19">
-        <v>45771</v>
+        <v>45775</v>
       </c>
       <c r="C11" s="21">
         <v>0.375</v>
@@ -972,7 +1019,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="19">
-        <v>45772</v>
+        <v>45776</v>
       </c>
       <c r="D12" s="21">
         <v>0.375</v>
@@ -992,7 +1039,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="19">
-        <v>45771</v>
+        <v>45775</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="25">
@@ -1008,26 +1055,64 @@
         <v>89543512312</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="27">
         <v>45770</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="28">
         <v>0.375</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="30">
         <v>89543512312</v>
       </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="2">
+        <v>89321728526</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="2">
+        <v>89178264458</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="31"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>